<commit_message>
adding compatibility for python 2
</commit_message>
<xml_diff>
--- a/projects/puerto_rico_stoch/data/data_U.xlsx
+++ b/projects/puerto_rico_stoch/data/data_U.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBB6CD6-999B-4AD7-AC2F-9C6C2CC1AA1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="941" activeTab="8"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -24,17 +25,23 @@
     <sheet name="ReserveMargin" sheetId="13" r:id="rId15"/>
     <sheet name="capacityFactorTOD" sheetId="14" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="220">
   <si>
     <t>connection</t>
   </si>
@@ -699,7 +706,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1104,19 +1111,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1136,7 +1143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1156,7 +1163,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -1164,7 +1171,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -1172,7 +1179,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -1183,7 +1190,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -1191,7 +1198,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -1202,7 +1209,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1210,7 +1217,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>92</v>
       </c>
@@ -1218,7 +1225,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -1226,7 +1233,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -1240,7 +1247,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>136</v>
       </c>
@@ -1248,7 +1255,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -1256,7 +1263,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -1264,7 +1271,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -1272,7 +1279,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -1280,7 +1287,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>141</v>
       </c>
@@ -1288,7 +1295,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -1296,7 +1303,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>143</v>
       </c>
@@ -1304,7 +1311,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>144</v>
       </c>
@@ -1312,7 +1319,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>145</v>
       </c>
@@ -1320,7 +1327,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>171</v>
       </c>
@@ -1328,7 +1335,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>146</v>
       </c>
@@ -1336,7 +1343,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>149</v>
       </c>
@@ -1344,7 +1351,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>196</v>
       </c>
@@ -1354,38 +1361,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1"/>
-    <hyperlink ref="E7" r:id="rId2"/>
-    <hyperlink ref="E8" r:id="rId3"/>
-    <hyperlink ref="E10" r:id="rId4"/>
-    <hyperlink ref="E18" r:id="rId5"/>
-    <hyperlink ref="E17" r:id="rId6"/>
-    <hyperlink ref="E16" r:id="rId7"/>
-    <hyperlink ref="E20" r:id="rId8"/>
-    <hyperlink ref="E21" r:id="rId9"/>
-    <hyperlink ref="E23" r:id="rId10"/>
-    <hyperlink ref="E22" r:id="rId11"/>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E18" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E17" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E16" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E20" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E21" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E23" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E22" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -1411,7 +1418,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>70</v>
       </c>
@@ -1437,7 +1444,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>106</v>
       </c>
@@ -1463,7 +1470,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
@@ -1489,7 +1496,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>108</v>
       </c>
@@ -1515,7 +1522,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>109</v>
       </c>
@@ -1541,7 +1548,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>110</v>
       </c>
@@ -1567,7 +1574,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>111</v>
       </c>
@@ -1593,7 +1600,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>112</v>
       </c>
@@ -1619,7 +1626,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>113</v>
       </c>
@@ -1645,7 +1652,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>114</v>
       </c>
@@ -1671,7 +1678,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>115</v>
       </c>
@@ -1697,7 +1704,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>116</v>
       </c>
@@ -1723,7 +1730,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
         <v>117</v>
       </c>
@@ -1749,7 +1756,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
         <v>118</v>
       </c>
@@ -1775,7 +1782,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
         <v>215</v>
       </c>
@@ -1801,7 +1808,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
         <v>216</v>
       </c>
@@ -1827,7 +1834,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
         <v>218</v>
       </c>
@@ -1853,7 +1860,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
         <v>119</v>
       </c>
@@ -1879,7 +1886,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
         <v>120</v>
       </c>
@@ -1905,7 +1912,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="23" t="s">
         <v>121</v>
       </c>
@@ -1931,7 +1938,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="23" t="s">
         <v>122</v>
       </c>
@@ -1957,7 +1964,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>131</v>
       </c>
@@ -1983,7 +1990,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>132</v>
       </c>
@@ -2009,7 +2016,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>194</v>
       </c>
@@ -2035,7 +2042,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>133</v>
       </c>
@@ -2061,7 +2068,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>134</v>
       </c>
@@ -2087,7 +2094,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>135</v>
       </c>
@@ -2130,25 +2137,25 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
@@ -2177,7 +2184,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>69</v>
       </c>
@@ -2206,7 +2213,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>106</v>
       </c>
@@ -2231,7 +2238,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
@@ -2254,7 +2261,7 @@
       </c>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>108</v>
       </c>
@@ -2277,7 +2284,7 @@
       </c>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>109</v>
       </c>
@@ -2300,7 +2307,7 @@
       </c>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>110</v>
       </c>
@@ -2323,7 +2330,7 @@
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>111</v>
       </c>
@@ -2346,7 +2353,7 @@
       </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>112</v>
       </c>
@@ -2371,7 +2378,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>113</v>
       </c>
@@ -2396,7 +2403,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>114</v>
       </c>
@@ -2421,7 +2428,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>115</v>
       </c>
@@ -2446,7 +2453,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>116</v>
       </c>
@@ -2471,7 +2478,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
         <v>117</v>
       </c>
@@ -2494,7 +2501,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
         <v>118</v>
       </c>
@@ -2519,7 +2526,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
         <v>215</v>
       </c>
@@ -2544,7 +2551,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
         <v>216</v>
       </c>
@@ -2569,7 +2576,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
         <v>218</v>
       </c>
@@ -2594,7 +2601,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
         <v>119</v>
       </c>
@@ -2619,7 +2626,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
         <v>120</v>
       </c>
@@ -2644,7 +2651,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="23" t="s">
         <v>121</v>
       </c>
@@ -2669,7 +2676,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="23" t="s">
         <v>122</v>
       </c>
@@ -2694,7 +2701,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>131</v>
       </c>
@@ -2717,7 +2724,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>132</v>
       </c>
@@ -2742,7 +2749,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>194</v>
       </c>
@@ -2767,7 +2774,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>133</v>
       </c>
@@ -2792,7 +2799,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>134</v>
       </c>
@@ -2817,7 +2824,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>135</v>
       </c>
@@ -2849,25 +2856,25 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -2890,7 +2897,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -2913,7 +2920,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>106</v>
       </c>
@@ -2932,7 +2939,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
@@ -2951,7 +2958,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>108</v>
       </c>
@@ -2970,7 +2977,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>109</v>
       </c>
@@ -2989,7 +2996,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>110</v>
       </c>
@@ -3008,7 +3015,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>111</v>
       </c>
@@ -3027,7 +3034,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>112</v>
       </c>
@@ -3050,7 +3057,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>113</v>
       </c>
@@ -3069,7 +3076,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>114</v>
       </c>
@@ -3088,7 +3095,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>115</v>
       </c>
@@ -3107,7 +3114,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>116</v>
       </c>
@@ -3126,7 +3133,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
         <v>117</v>
       </c>
@@ -3149,7 +3156,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
         <v>118</v>
       </c>
@@ -3172,7 +3179,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
         <v>215</v>
       </c>
@@ -3195,7 +3202,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
         <v>216</v>
       </c>
@@ -3216,7 +3223,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
         <v>218</v>
       </c>
@@ -3237,7 +3244,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
         <v>119</v>
       </c>
@@ -3260,7 +3267,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
         <v>120</v>
       </c>
@@ -3283,7 +3290,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="23" t="s">
         <v>121</v>
       </c>
@@ -3306,7 +3313,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="23" t="s">
         <v>122</v>
       </c>
@@ -3329,7 +3336,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>131</v>
       </c>
@@ -3352,7 +3359,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>132</v>
       </c>
@@ -3375,7 +3382,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>194</v>
       </c>
@@ -3398,7 +3405,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>133</v>
       </c>
@@ -3421,7 +3428,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>134</v>
       </c>
@@ -3444,7 +3451,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>135</v>
       </c>
@@ -3467,7 +3474,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F29" s="7"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
@@ -3480,25 +3487,25 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21:F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -3521,7 +3528,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -3544,7 +3551,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>106</v>
       </c>
@@ -3555,7 +3562,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
@@ -3566,7 +3573,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>108</v>
       </c>
@@ -3577,7 +3584,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>109</v>
       </c>
@@ -3588,7 +3595,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>110</v>
       </c>
@@ -3599,7 +3606,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>111</v>
       </c>
@@ -3610,7 +3617,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>112</v>
       </c>
@@ -3623,35 +3630,35 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>113</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>114</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>115</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>116</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
         <v>117</v>
       </c>
@@ -3662,7 +3669,7 @@
       <c r="F14" s="26"/>
       <c r="G14" s="26"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
         <v>118</v>
       </c>
@@ -3677,7 +3684,7 @@
       <c r="F15" s="26"/>
       <c r="G15" s="26"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
         <v>215</v>
       </c>
@@ -3692,7 +3699,7 @@
       <c r="F16" s="26"/>
       <c r="G16" s="26"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
         <v>216</v>
       </c>
@@ -3707,7 +3714,7 @@
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
         <v>218</v>
       </c>
@@ -3722,7 +3729,7 @@
       <c r="F18" s="26"/>
       <c r="G18" s="26"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
         <v>119</v>
       </c>
@@ -3737,7 +3744,7 @@
       <c r="F19" s="26"/>
       <c r="G19" s="26"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
         <v>120</v>
       </c>
@@ -3748,7 +3755,7 @@
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="23" t="s">
         <v>121</v>
       </c>
@@ -3761,7 +3768,7 @@
       </c>
       <c r="G21" s="26"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="23" t="s">
         <v>122</v>
       </c>
@@ -3774,12 +3781,12 @@
       </c>
       <c r="G22" s="26"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>132</v>
       </c>
@@ -3790,7 +3797,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>194</v>
       </c>
@@ -3801,12 +3808,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>134</v>
       </c>
@@ -3814,7 +3821,7 @@
         <v>705.6</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>135</v>
       </c>
@@ -3829,21 +3836,21 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S37" sqref="S37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -3857,7 +3864,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -3871,7 +3878,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>106</v>
       </c>
@@ -3885,7 +3892,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
@@ -3899,7 +3906,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>107</v>
       </c>
@@ -3913,7 +3920,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>107</v>
       </c>
@@ -3927,7 +3934,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>108</v>
       </c>
@@ -3941,7 +3948,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>108</v>
       </c>
@@ -3955,7 +3962,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>108</v>
       </c>
@@ -3969,7 +3976,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>109</v>
       </c>
@@ -3983,7 +3990,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>110</v>
       </c>
@@ -3997,7 +4004,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>110</v>
       </c>
@@ -4011,7 +4018,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>110</v>
       </c>
@@ -4025,7 +4032,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>110</v>
       </c>
@@ -4039,7 +4046,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>111</v>
       </c>
@@ -4053,7 +4060,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>111</v>
       </c>
@@ -4067,7 +4074,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>111</v>
       </c>
@@ -4081,7 +4088,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>111</v>
       </c>
@@ -4095,7 +4102,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>111</v>
       </c>
@@ -4109,7 +4116,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>111</v>
       </c>
@@ -4123,7 +4130,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>112</v>
       </c>
@@ -4137,7 +4144,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>113</v>
       </c>
@@ -4151,7 +4158,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>114</v>
       </c>
@@ -4165,7 +4172,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>115</v>
       </c>
@@ -4179,7 +4186,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>115</v>
       </c>
@@ -4193,7 +4200,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>116</v>
       </c>
@@ -4214,21 +4221,21 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
@@ -4236,7 +4243,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -4244,7 +4251,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -4255,22 +4262,22 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -4287,7 +4294,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -4304,7 +4311,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>95</v>
       </c>
@@ -4321,7 +4328,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>95</v>
       </c>
@@ -4338,7 +4345,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>95</v>
       </c>
@@ -4355,7 +4362,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>95</v>
       </c>
@@ -4372,7 +4379,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>95</v>
       </c>
@@ -4389,7 +4396,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>95</v>
       </c>
@@ -4406,7 +4413,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>95</v>
       </c>
@@ -4423,7 +4430,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>95</v>
       </c>
@@ -4440,7 +4447,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>95</v>
       </c>
@@ -4457,7 +4464,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>95</v>
       </c>
@@ -4474,7 +4481,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>95</v>
       </c>
@@ -4491,7 +4498,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>95</v>
       </c>
@@ -4508,7 +4515,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>95</v>
       </c>
@@ -4525,7 +4532,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>95</v>
       </c>
@@ -4542,7 +4549,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>95</v>
       </c>
@@ -4559,7 +4566,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>95</v>
       </c>
@@ -4576,7 +4583,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>95</v>
       </c>
@@ -4593,7 +4600,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>95</v>
       </c>
@@ -4610,7 +4617,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>95</v>
       </c>
@@ -4627,7 +4634,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>95</v>
       </c>
@@ -4644,7 +4651,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>95</v>
       </c>
@@ -4661,7 +4668,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>95</v>
       </c>
@@ -4678,7 +4685,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>95</v>
       </c>
@@ -4695,7 +4702,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>95</v>
       </c>
@@ -4712,7 +4719,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>95</v>
       </c>
@@ -4729,7 +4736,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>95</v>
       </c>
@@ -4746,7 +4753,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>95</v>
       </c>
@@ -4763,7 +4770,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>95</v>
       </c>
@@ -4780,7 +4787,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>95</v>
       </c>
@@ -4797,7 +4804,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>95</v>
       </c>
@@ -4814,7 +4821,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>95</v>
       </c>
@@ -4831,7 +4838,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>95</v>
       </c>
@@ -4848,7 +4855,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>95</v>
       </c>
@@ -4865,7 +4872,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>95</v>
       </c>
@@ -4882,7 +4889,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>95</v>
       </c>
@@ -4899,7 +4906,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>95</v>
       </c>
@@ -4916,7 +4923,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>95</v>
       </c>
@@ -4933,7 +4940,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>95</v>
       </c>
@@ -4950,7 +4957,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>95</v>
       </c>
@@ -4967,7 +4974,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>95</v>
       </c>
@@ -4984,7 +4991,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>95</v>
       </c>
@@ -5001,7 +5008,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>95</v>
       </c>
@@ -5018,7 +5025,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>95</v>
       </c>
@@ -5035,7 +5042,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>95</v>
       </c>
@@ -5052,7 +5059,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>95</v>
       </c>
@@ -5069,7 +5076,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>95</v>
       </c>
@@ -5086,7 +5093,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>95</v>
       </c>
@@ -5103,7 +5110,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>95</v>
       </c>
@@ -5120,7 +5127,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>96</v>
       </c>
@@ -5137,7 +5144,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>96</v>
       </c>
@@ -5154,7 +5161,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>96</v>
       </c>
@@ -5171,7 +5178,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>96</v>
       </c>
@@ -5188,7 +5195,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>96</v>
       </c>
@@ -5205,7 +5212,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>96</v>
       </c>
@@ -5222,7 +5229,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>96</v>
       </c>
@@ -5239,7 +5246,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>96</v>
       </c>
@@ -5256,7 +5263,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>96</v>
       </c>
@@ -5273,7 +5280,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>96</v>
       </c>
@@ -5290,7 +5297,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>96</v>
       </c>
@@ -5307,7 +5314,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>96</v>
       </c>
@@ -5324,7 +5331,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>96</v>
       </c>
@@ -5341,7 +5348,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>96</v>
       </c>
@@ -5358,7 +5365,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>96</v>
       </c>
@@ -5375,7 +5382,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>96</v>
       </c>
@@ -5392,7 +5399,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>96</v>
       </c>
@@ -5409,7 +5416,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>96</v>
       </c>
@@ -5426,7 +5433,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>96</v>
       </c>
@@ -5443,7 +5450,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>96</v>
       </c>
@@ -5460,7 +5467,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>96</v>
       </c>
@@ -5477,7 +5484,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>96</v>
       </c>
@@ -5494,7 +5501,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>96</v>
       </c>
@@ -5511,7 +5518,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>96</v>
       </c>
@@ -5528,7 +5535,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>96</v>
       </c>
@@ -5545,7 +5552,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>96</v>
       </c>
@@ -5562,7 +5569,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>96</v>
       </c>
@@ -5579,7 +5586,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>96</v>
       </c>
@@ -5596,7 +5603,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>96</v>
       </c>
@@ -5613,7 +5620,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>96</v>
       </c>
@@ -5630,7 +5637,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>96</v>
       </c>
@@ -5647,7 +5654,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>96</v>
       </c>
@@ -5664,7 +5671,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>96</v>
       </c>
@@ -5681,7 +5688,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>96</v>
       </c>
@@ -5698,7 +5705,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>96</v>
       </c>
@@ -5715,7 +5722,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>96</v>
       </c>
@@ -5732,7 +5739,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>96</v>
       </c>
@@ -5749,7 +5756,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>96</v>
       </c>
@@ -5766,7 +5773,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>96</v>
       </c>
@@ -5783,7 +5790,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>96</v>
       </c>
@@ -5800,7 +5807,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>96</v>
       </c>
@@ -5817,7 +5824,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>96</v>
       </c>
@@ -5834,7 +5841,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>96</v>
       </c>
@@ -5851,7 +5858,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>96</v>
       </c>
@@ -5868,7 +5875,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>96</v>
       </c>
@@ -5885,7 +5892,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>96</v>
       </c>
@@ -5902,7 +5909,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>96</v>
       </c>
@@ -5919,7 +5926,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>96</v>
       </c>
@@ -5943,18 +5950,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
@@ -5965,7 +5972,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -5976,7 +5983,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -5987,7 +5994,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -6004,20 +6011,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -6028,7 +6035,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -6039,7 +6046,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>185</v>
       </c>
@@ -6050,7 +6057,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>186</v>
       </c>
@@ -6061,7 +6068,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>187</v>
       </c>
@@ -6072,7 +6079,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>188</v>
       </c>
@@ -6083,7 +6090,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>189</v>
       </c>
@@ -6094,7 +6101,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>190</v>
       </c>
@@ -6105,7 +6112,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>191</v>
       </c>
@@ -6116,7 +6123,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>192</v>
       </c>
@@ -6127,7 +6134,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>193</v>
       </c>
@@ -6138,7 +6145,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -6149,7 +6156,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -6160,7 +6167,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -6171,7 +6178,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -6182,7 +6189,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -6193,7 +6200,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -6204,7 +6211,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -6215,7 +6222,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -6226,7 +6233,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -6237,7 +6244,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -6248,7 +6255,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -6259,7 +6266,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -6270,7 +6277,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -6281,7 +6288,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -6292,7 +6299,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -6310,26 +6317,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6364,7 +6371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -6399,7 +6406,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -6434,7 +6441,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>197</v>
       </c>
@@ -6465,7 +6472,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>202</v>
       </c>
@@ -6500,7 +6507,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>203</v>
       </c>
@@ -6535,7 +6542,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -6555,7 +6562,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>201</v>
       </c>
@@ -6590,7 +6597,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>200</v>
       </c>
@@ -6625,7 +6632,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>205</v>
       </c>
@@ -6648,7 +6655,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>206</v>
       </c>
@@ -6671,7 +6678,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>213</v>
       </c>
@@ -6694,7 +6701,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>207</v>
       </c>
@@ -6717,7 +6724,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>208</v>
       </c>
@@ -6747,20 +6754,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6774,7 +6781,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -6788,7 +6795,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -6802,7 +6809,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>197</v>
       </c>
@@ -6816,7 +6823,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>203</v>
       </c>
@@ -6830,7 +6837,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>202</v>
       </c>
@@ -6851,20 +6858,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -6878,7 +6885,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -6892,7 +6899,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2016</v>
       </c>
@@ -6902,9 +6909,11 @@
       <c r="C3" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -6914,9 +6923,11 @@
       <c r="C4" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2026</v>
       </c>
@@ -6926,39 +6937,18 @@
       <c r="C5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2031</v>
-      </c>
-      <c r="B6" s="3">
-        <v>65.77</v>
-      </c>
-      <c r="C6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2036</v>
-      </c>
-      <c r="B7" s="3">
-        <v>65.47</v>
-      </c>
-      <c r="C7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2041</v>
-      </c>
-      <c r="B8" s="3">
-        <v>65.41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>87</v>
-      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6967,20 +6957,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
@@ -6988,7 +6978,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -6996,7 +6986,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.09</v>
       </c>
@@ -7010,28 +7000,28 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -7069,7 +7059,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -7107,7 +7097,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -7134,7 +7124,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -7163,7 +7153,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -7192,7 +7182,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -7206,7 +7196,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -7226,7 +7216,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -7255,7 +7245,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -7287,7 +7277,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -7301,7 +7291,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -7322,20 +7312,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -7349,7 +7339,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -7363,7 +7353,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
expanded scenarios and post processing
</commit_message>
<xml_diff>
--- a/projects/puerto_rico_stoch/data/data_U.xlsx
+++ b/projects/puerto_rico_stoch/data/data_U.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D3F4A9-067A-4ECC-A741-72103BB6DE90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD96010-C644-4A0B-B39D-59C12367FB15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="941" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -3558,7 +3558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -5346,10 +5346,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5358,7 +5358,7 @@
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>185</v>
       </c>
@@ -5390,12 +5390,8 @@
       <c r="C3">
         <v>4.1667000000000003E-2</v>
       </c>
-      <c r="E3">
-        <f>MAX(B3:B26)</f>
-        <v>4.7E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>186</v>
       </c>
@@ -5406,7 +5402,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>187</v>
       </c>
@@ -5417,7 +5413,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>188</v>
       </c>
@@ -5428,7 +5424,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>189</v>
       </c>
@@ -5439,7 +5435,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>190</v>
       </c>
@@ -5450,7 +5446,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>191</v>
       </c>
@@ -5461,7 +5457,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>192</v>
       </c>
@@ -5472,7 +5468,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>193</v>
       </c>
@@ -5483,7 +5479,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -5494,7 +5490,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -5505,7 +5501,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -5516,7 +5512,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -5527,7 +5523,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>53</v>
       </c>

</xml_diff>